<commit_message>
atualização do projeto Gestao Versus para utilizar o Chat GPT
</commit_message>
<xml_diff>
--- a/Suporte/Esquema Banco de Dados Versus.xlsx
+++ b/Suporte/Esquema Banco de Dados Versus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GestaoVersus\Arquivos_suporte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GestaoVersus\Suporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2931DB-710C-42BE-B786-861EABEC7210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF2760C-F4C2-4DE0-A76E-89AEFECAE2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E01C0C5-C9CE-4DBC-9B28-6400CEDA22BE}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0E01C0C5-C9CE-4DBC-9B28-6400CEDA22BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastros" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>PRC_ATIV_OBS</t>
   </si>
   <si>
-    <t>PRC_ATIV_TIME_EXECUTOR_ID</t>
-  </si>
-  <si>
     <t>PRJ_GESTAO</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>GER_USU_SENHA</t>
+  </si>
+  <si>
+    <t>PRC_ATIV_TIME_ID</t>
   </si>
 </sst>
 </file>
@@ -290,7 +290,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +300,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,11 +343,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,8 +688,8 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,13 +713,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -716,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -725,7 +739,7 @@
         <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -733,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -742,7 +756,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -750,7 +764,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -761,10 +775,10 @@
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -773,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -781,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -790,7 +804,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -798,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7">
         <v>256</v>
@@ -807,7 +821,7 @@
         <v>256</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -815,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8">
         <v>256</v>
@@ -829,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>999</v>
@@ -839,11 +853,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -857,7 +871,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11">
         <v>999</v>
@@ -867,11 +881,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -881,11 +895,11 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -895,11 +909,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -909,11 +923,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -923,11 +937,11 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -937,11 +951,11 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -951,11 +965,11 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>65</v>
+      <c r="B18" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -965,11 +979,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -979,11 +993,11 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -993,11 +1007,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1007,11 +1021,11 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1021,11 +1035,11 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1035,11 +1049,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1050,29 +1064,29 @@
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1098,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1093,7 +1107,7 @@
         <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1101,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1110,15 +1124,15 @@
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31">
         <v>20</v>
@@ -1127,7 +1141,7 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1135,7 +1149,7 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>256</v>
@@ -1144,7 +1158,7 @@
         <v>256</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1152,7 +1166,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33">
         <v>256</v>
@@ -1166,7 +1180,7 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34">
         <v>999</v>
@@ -1177,10 +1191,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1191,40 +1205,40 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
         <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1233,15 +1247,15 @@
         <v>24</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41">
         <v>20</v>
@@ -1250,15 +1264,15 @@
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1269,10 +1283,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D43">
         <v>3</v>
@@ -1281,15 +1295,15 @@
         <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D44">
         <v>20</v>
@@ -1298,15 +1312,15 @@
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45">
         <v>256</v>
@@ -1315,15 +1329,15 @@
         <v>256</v>
       </c>
       <c r="F45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46">
         <v>999</v>
@@ -1334,10 +1348,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -1348,10 +1362,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -1362,10 +1376,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49">
         <v>3</v>
@@ -1376,10 +1390,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50">
         <v>256</v>
@@ -1390,10 +1404,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D51">
         <v>999</v>
@@ -1404,56 +1418,56 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
         <v>56</v>
-      </c>
-      <c r="C56" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="s">
         <v>66</v>
       </c>
-      <c r="B58" t="s">
-        <v>67</v>
-      </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -1462,15 +1476,15 @@
         <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D59">
         <v>256</v>
@@ -1479,15 +1493,15 @@
         <v>256</v>
       </c>
       <c r="F59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60">
         <v>256</v>
@@ -1496,20 +1510,20 @@
         <v>256</v>
       </c>
       <c r="F60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D62">
         <v>256</v>
@@ -1520,10 +1534,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D63">
         <v>256</v>
@@ -1534,10 +1548,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D64">
         <v>999</v>
@@ -1548,29 +1562,29 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>